<commit_message>
modified lls pharmacy, patient, cpr patient,
let c
</commit_message>
<xml_diff>
--- a/QA/testcases/LLS/Pharmacy/L_Phar_Patient_App_Create__Denied.xlsx
+++ b/QA/testcases/LLS/Pharmacy/L_Phar_Patient_App_Create__Denied.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27465" windowHeight="13230"/>
+    <workbookView windowWidth="28680" windowHeight="13650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324">
   <si>
     <t>Step No</t>
   </si>
@@ -574,45 +574,6 @@
   </si>
   <si>
     <t>LLS_T_SETTING</t>
-  </si>
-  <si>
-    <t>MEDICATION_NAME</t>
-  </si>
-  <si>
-    <t>Type Medication name</t>
-  </si>
-  <si>
-    <t>Medication name entered</t>
-  </si>
-  <si>
-    <t>Select Medication name</t>
-  </si>
-  <si>
-    <t>Medication name selected</t>
-  </si>
-  <si>
-    <t>DOSAGE</t>
-  </si>
-  <si>
-    <t>TestDosage</t>
-  </si>
-  <si>
-    <t>Enter Dosage</t>
-  </si>
-  <si>
-    <t>Dosage entered</t>
-  </si>
-  <si>
-    <t>FREQUENCY</t>
-  </si>
-  <si>
-    <t>Daily</t>
-  </si>
-  <si>
-    <t>Enter frequency</t>
-  </si>
-  <si>
-    <t>Frequency entered</t>
   </si>
   <si>
     <t>AGREE_SUBMIT_BUTTON</t>
@@ -1049,10 +1010,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -1091,22 +1052,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1121,46 +1074,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1172,17 +1098,45 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1198,27 +1152,34 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1261,61 +1222,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1333,7 +1240,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1345,7 +1276,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1357,43 +1384,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1411,37 +1402,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1505,17 +1466,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1544,17 +1505,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1574,20 +1538,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1605,7 +1566,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1623,130 +1584,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2201,10 +2162,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H118"/>
+  <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81:A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -3925,7 +3886,7 @@
       <c r="H81" s="17"/>
     </row>
     <row r="82" spans="1:8">
-      <c r="A82" s="8">
+      <c r="A82" s="11">
         <v>81</v>
       </c>
       <c r="B82" s="10" t="s">
@@ -3946,755 +3907,649 @@
       <c r="A83" s="11">
         <v>82</v>
       </c>
-      <c r="B83" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C83" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D83" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="E83" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="F83" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="G83" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="H83" s="17"/>
+      <c r="B83" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D83" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E83" s="10"/>
+      <c r="F83" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G83" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="H83" s="9"/>
     </row>
     <row r="84" spans="1:8">
-      <c r="A84" s="8">
+      <c r="A84" s="11">
         <v>83</v>
       </c>
-      <c r="B84" s="10" t="s">
+      <c r="B84" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C84" s="10"/>
-      <c r="D84" s="10"/>
-      <c r="E84" s="10">
-        <v>5</v>
-      </c>
-      <c r="F84" s="10"/>
-      <c r="G84" s="10"/>
-      <c r="H84" s="9"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12">
+        <v>4</v>
+      </c>
+      <c r="F84" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G84" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H84" s="17"/>
     </row>
     <row r="85" spans="1:8">
       <c r="A85" s="11">
         <v>84</v>
       </c>
-      <c r="B85" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="C85" s="12"/>
-      <c r="D85" s="12"/>
-      <c r="E85" s="12"/>
-      <c r="F85" s="12" t="s">
+      <c r="B85" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D85" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E85" s="10"/>
+      <c r="F85" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="G85" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="H85" s="9"/>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="11">
+        <v>85</v>
+      </c>
+      <c r="B86" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C86" s="12"/>
+      <c r="D86" s="12"/>
+      <c r="E86" s="12">
+        <v>2</v>
+      </c>
+      <c r="F86" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="G85" s="12" t="s">
+      <c r="G86" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="H85" s="17"/>
-    </row>
-    <row r="86" spans="1:8">
-      <c r="A86" s="8">
-        <v>85</v>
-      </c>
-      <c r="B86" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C86" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D86" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="E86" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="F86" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="G86" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="H86" s="9"/>
+      <c r="H86" s="17"/>
     </row>
     <row r="87" spans="1:8">
       <c r="A87" s="11">
         <v>86</v>
       </c>
-      <c r="B87" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C87" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D87" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="E87" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="F87" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="G87" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="H87" s="17"/>
+      <c r="B87" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C87" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D87" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="E87" s="10"/>
+      <c r="F87" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="G87" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="H87" s="9"/>
     </row>
     <row r="88" spans="1:8">
-      <c r="A88" s="8">
+      <c r="A88" s="11">
         <v>87</v>
       </c>
-      <c r="B88" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C88" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D88" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="E88" s="10"/>
-      <c r="F88" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="G88" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H88" s="9"/>
+      <c r="B88" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C88" s="12"/>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12">
+        <v>2</v>
+      </c>
+      <c r="F88" s="12"/>
+      <c r="G88" s="12"/>
+      <c r="H88" s="17"/>
     </row>
     <row r="89" spans="1:8">
       <c r="A89" s="11">
         <v>88</v>
       </c>
-      <c r="B89" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C89" s="12"/>
-      <c r="D89" s="12"/>
-      <c r="E89" s="12">
-        <v>4</v>
-      </c>
-      <c r="F89" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G89" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H89" s="17"/>
+      <c r="B89" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C89" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D89" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="E89" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="F89" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="G89" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="H89" s="9"/>
     </row>
     <row r="90" spans="1:8">
-      <c r="A90" s="8">
+      <c r="A90" s="11">
         <v>89</v>
       </c>
-      <c r="B90" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C90" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D90" s="10" t="s">
+      <c r="B90" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C90" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D90" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="E90" s="10"/>
-      <c r="F90" s="10" t="s">
+      <c r="E90" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="G90" s="10" t="s">
+      <c r="F90" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="H90" s="9"/>
+      <c r="G90" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="H90" s="17"/>
     </row>
     <row r="91" spans="1:8">
       <c r="A91" s="11">
         <v>90</v>
       </c>
-      <c r="B91" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C91" s="12"/>
-      <c r="D91" s="12"/>
-      <c r="E91" s="12">
-        <v>2</v>
-      </c>
-      <c r="F91" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="G91" s="12" t="s">
+      <c r="B91" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="H91" s="17"/>
+      <c r="C91" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D91" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="E91" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="F91" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="G91" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="H91" s="9"/>
     </row>
     <row r="92" spans="1:8">
-      <c r="A92" s="8">
+      <c r="A92" s="11">
         <v>91</v>
       </c>
-      <c r="B92" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="C92" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D92" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="E92" s="10"/>
-      <c r="F92" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="G92" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="H92" s="9"/>
+      <c r="B92" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C92" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D92" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E92" s="12"/>
+      <c r="F92" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="G92" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="H92" s="17"/>
     </row>
     <row r="93" spans="1:8">
       <c r="A93" s="11">
         <v>92</v>
       </c>
-      <c r="B93" s="12" t="s">
+      <c r="B93" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C93" s="12"/>
-      <c r="D93" s="12"/>
-      <c r="E93" s="12">
-        <v>2</v>
-      </c>
-      <c r="F93" s="12"/>
-      <c r="G93" s="12"/>
-      <c r="H93" s="17"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="13"/>
+      <c r="E93" s="10">
+        <v>4</v>
+      </c>
+      <c r="F93" s="10"/>
+      <c r="G93" s="10"/>
+      <c r="H93" s="9"/>
     </row>
     <row r="94" spans="1:8">
-      <c r="A94" s="8">
+      <c r="A94" s="11">
         <v>93</v>
       </c>
-      <c r="B94" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C94" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D94" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="E94" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="F94" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="G94" s="10" t="s">
+      <c r="B94" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C94" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D94" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="H94" s="9"/>
+      <c r="E94" s="12"/>
+      <c r="F94" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="G94" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="H94" s="17"/>
     </row>
     <row r="95" spans="1:8">
       <c r="A95" s="11">
         <v>94</v>
       </c>
-      <c r="B95" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C95" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D95" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E95" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="F95" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="G95" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="H95" s="17"/>
+      <c r="B95" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C95" s="10"/>
+      <c r="D95" s="10"/>
+      <c r="E95" s="10">
+        <v>5</v>
+      </c>
+      <c r="F95" s="10"/>
+      <c r="G95" s="10"/>
+      <c r="H95" s="9"/>
     </row>
     <row r="96" spans="1:8">
-      <c r="A96" s="8">
+      <c r="A96" s="11">
         <v>95</v>
       </c>
-      <c r="B96" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="C96" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D96" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="E96" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="F96" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="G96" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="H96" s="9"/>
+      <c r="B96" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C96" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D96" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E96" s="12"/>
+      <c r="F96" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G96" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H96" s="19">
+        <v>3</v>
+      </c>
     </row>
     <row r="97" spans="1:8">
       <c r="A97" s="11">
         <v>96</v>
       </c>
-      <c r="B97" s="12" t="s">
+      <c r="B97" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C97" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D97" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="E97" s="12"/>
-      <c r="F97" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="G97" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="H97" s="17"/>
+      <c r="C97" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D97" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E97" s="10"/>
+      <c r="F97" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G97" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H97" s="19"/>
     </row>
     <row r="98" spans="1:8">
-      <c r="A98" s="8">
+      <c r="A98" s="11">
         <v>97</v>
       </c>
       <c r="B98" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C98" s="10"/>
-      <c r="D98" s="13"/>
+      <c r="D98" s="10"/>
       <c r="E98" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F98" s="10"/>
       <c r="G98" s="10"/>
-      <c r="H98" s="9"/>
+      <c r="H98" s="19"/>
     </row>
     <row r="99" spans="1:8">
       <c r="A99" s="11">
         <v>98</v>
       </c>
-      <c r="B99" s="12" t="s">
+      <c r="B99" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C99" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D99" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="E99" s="12"/>
-      <c r="F99" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="G99" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="H99" s="17"/>
+      <c r="C99" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D99" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="E99" s="18"/>
+      <c r="F99" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="G99" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="H99" s="18"/>
     </row>
     <row r="100" spans="1:8">
-      <c r="A100" s="8">
+      <c r="A100" s="11">
         <v>99</v>
       </c>
-      <c r="B100" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C100" s="10"/>
-      <c r="D100" s="10"/>
-      <c r="E100" s="10">
-        <v>5</v>
-      </c>
-      <c r="F100" s="10"/>
-      <c r="G100" s="10"/>
-      <c r="H100" s="9"/>
+      <c r="B100" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C100" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D100" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="E100" s="21"/>
+      <c r="F100" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="G100" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="H100" s="21"/>
     </row>
     <row r="101" spans="1:8">
       <c r="A101" s="11">
         <v>100</v>
       </c>
       <c r="B101" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C101" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D101" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E101" s="12"/>
-      <c r="F101" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G101" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H101" s="19">
-        <v>3</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C101" s="18"/>
+      <c r="D101" s="18"/>
+      <c r="E101" s="18">
+        <v>20</v>
+      </c>
+      <c r="F101" s="18"/>
+      <c r="G101" s="18"/>
+      <c r="H101" s="18"/>
     </row>
     <row r="102" spans="1:8">
-      <c r="A102" s="8">
+      <c r="A102" s="11">
         <v>101</v>
       </c>
-      <c r="B102" s="10" t="s">
+      <c r="B102" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C102" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D102" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E102" s="10"/>
-      <c r="F102" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G102" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H102" s="19"/>
+      <c r="C102" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D102" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="E102" s="21"/>
+      <c r="F102" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="G102" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="H102" s="21"/>
     </row>
     <row r="103" spans="1:8">
       <c r="A103" s="11">
         <v>102</v>
       </c>
-      <c r="B103" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C103" s="10"/>
-      <c r="D103" s="10"/>
-      <c r="E103" s="10">
-        <v>5</v>
-      </c>
-      <c r="F103" s="10"/>
-      <c r="G103" s="10"/>
-      <c r="H103" s="19"/>
+      <c r="B103" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C103" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D103" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="E103" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="F103" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="G103" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="H103" s="18"/>
     </row>
     <row r="104" spans="1:8">
-      <c r="A104" s="8">
+      <c r="A104" s="11">
         <v>103</v>
       </c>
-      <c r="B104" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C104" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D104" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="E104" s="18"/>
-      <c r="F104" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="G104" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="H104" s="18"/>
+      <c r="B104" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C104" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D104" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="E104" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="F104" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="G104" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="H104" s="21"/>
     </row>
     <row r="105" spans="1:8">
       <c r="A105" s="11">
         <v>104</v>
       </c>
-      <c r="B105" s="21" t="s">
+      <c r="B105" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="C105" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D105" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="E105" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="F105" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="G105" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="H105" s="18"/>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106" s="11">
+        <v>105</v>
+      </c>
+      <c r="B106" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C105" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D105" s="22" t="s">
-        <v>225</v>
-      </c>
-      <c r="E105" s="21"/>
-      <c r="F105" s="21" t="s">
-        <v>226</v>
-      </c>
-      <c r="G105" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="H105" s="21"/>
-    </row>
-    <row r="106" spans="1:8">
-      <c r="A106" s="8">
-        <v>105</v>
-      </c>
-      <c r="B106" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C106" s="18"/>
-      <c r="D106" s="18"/>
-      <c r="E106" s="18">
-        <v>20</v>
-      </c>
-      <c r="F106" s="18"/>
-      <c r="G106" s="18"/>
-      <c r="H106" s="18"/>
+      <c r="C106" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D106" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="E106" s="21"/>
+      <c r="F106" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="G106" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="H106" s="21"/>
     </row>
     <row r="107" spans="1:8">
       <c r="A107" s="11">
         <v>106</v>
       </c>
-      <c r="B107" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C107" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D107" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="E107" s="21"/>
-      <c r="F107" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="G107" s="21" t="s">
-        <v>230</v>
-      </c>
-      <c r="H107" s="21"/>
+      <c r="B107" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C107" s="18"/>
+      <c r="D107" s="18"/>
+      <c r="E107" s="18">
+        <v>20</v>
+      </c>
+      <c r="F107" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G107" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H107" s="18"/>
     </row>
     <row r="108" spans="1:8">
-      <c r="A108" s="8">
+      <c r="A108" s="11">
         <v>107</v>
       </c>
-      <c r="B108" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C108" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D108" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="E108" s="18" t="s">
-        <v>204</v>
-      </c>
-      <c r="F108" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="G108" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="H108" s="18"/>
+      <c r="B108" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="C108" s="21"/>
+      <c r="D108" s="21"/>
+      <c r="E108" s="21"/>
+      <c r="F108" s="21"/>
+      <c r="G108" s="21"/>
+      <c r="H108" s="21"/>
     </row>
     <row r="109" spans="1:8">
       <c r="A109" s="11">
         <v>108</v>
       </c>
-      <c r="B109" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C109" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D109" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="E109" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="F109" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="G109" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="H109" s="21"/>
+      <c r="B109" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C109" s="18"/>
+      <c r="D109" s="18"/>
+      <c r="E109" s="18">
+        <v>10</v>
+      </c>
+      <c r="F109" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G109" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H109" s="18"/>
     </row>
     <row r="110" spans="1:8">
-      <c r="A110" s="8">
+      <c r="A110" s="11">
         <v>109</v>
       </c>
-      <c r="B110" s="18" t="s">
-        <v>211</v>
-      </c>
-      <c r="C110" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D110" s="20" t="s">
-        <v>212</v>
-      </c>
-      <c r="E110" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="F110" s="18" t="s">
-        <v>214</v>
-      </c>
-      <c r="G110" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="H110" s="18"/>
+      <c r="B110" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C110" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D110" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="E110" s="21"/>
+      <c r="F110" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="G110" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="H110" s="21"/>
     </row>
     <row r="111" spans="1:8">
       <c r="A111" s="11">
         <v>110</v>
       </c>
-      <c r="B111" s="21" t="s">
+      <c r="B111" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C111" s="18"/>
+      <c r="D111" s="18"/>
+      <c r="E111" s="18">
+        <v>5</v>
+      </c>
+      <c r="F111" s="18"/>
+      <c r="G111" s="18"/>
+      <c r="H111" s="18"/>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="A112" s="11">
+        <v>111</v>
+      </c>
+      <c r="B112" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C111" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D111" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="E111" s="21"/>
-      <c r="F111" s="21" t="s">
-        <v>217</v>
-      </c>
-      <c r="G111" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="H111" s="21"/>
-    </row>
-    <row r="112" spans="1:8">
-      <c r="A112" s="8">
-        <v>111</v>
-      </c>
-      <c r="B112" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C112" s="18"/>
-      <c r="D112" s="18"/>
-      <c r="E112" s="18">
-        <v>20</v>
-      </c>
-      <c r="F112" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G112" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H112" s="18"/>
+      <c r="C112" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D112" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="E112" s="12"/>
+      <c r="F112" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="G112" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="H112" s="12"/>
     </row>
     <row r="113" spans="1:8">
       <c r="A113" s="11">
         <v>112</v>
       </c>
-      <c r="B113" s="21" t="s">
-        <v>231</v>
-      </c>
-      <c r="C113" s="21"/>
-      <c r="D113" s="21"/>
-      <c r="E113" s="21"/>
-      <c r="F113" s="21"/>
-      <c r="G113" s="21"/>
-      <c r="H113" s="21"/>
-    </row>
-    <row r="114" spans="1:8">
-      <c r="A114" s="8">
-        <v>113</v>
-      </c>
-      <c r="B114" s="18" t="s">
+      <c r="B113" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C114" s="18"/>
-      <c r="D114" s="18"/>
-      <c r="E114" s="18">
-        <v>10</v>
-      </c>
-      <c r="F114" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G114" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H114" s="18"/>
-    </row>
-    <row r="115" spans="1:8">
-      <c r="A115" s="11">
-        <v>114</v>
-      </c>
-      <c r="B115" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C115" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D115" s="22" t="s">
-        <v>232</v>
-      </c>
-      <c r="E115" s="21"/>
-      <c r="F115" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="G115" s="21" t="s">
-        <v>234</v>
-      </c>
-      <c r="H115" s="21"/>
-    </row>
-    <row r="116" spans="1:8">
-      <c r="A116" s="8">
-        <v>115</v>
-      </c>
-      <c r="B116" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C116" s="18"/>
-      <c r="D116" s="18"/>
-      <c r="E116" s="18">
-        <v>5</v>
-      </c>
-      <c r="F116" s="18"/>
-      <c r="G116" s="18"/>
-      <c r="H116" s="18"/>
-    </row>
-    <row r="117" spans="1:8">
-      <c r="A117" s="11">
-        <v>116</v>
-      </c>
-      <c r="B117" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C117" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D117" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="E117" s="12"/>
-      <c r="F117" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="G117" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="H117" s="12"/>
-    </row>
-    <row r="118" spans="1:8">
-      <c r="A118" s="8">
-        <v>117</v>
-      </c>
-      <c r="B118" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C118" s="10"/>
-      <c r="D118" s="10"/>
-      <c r="E118" s="10">
+      <c r="C113" s="10"/>
+      <c r="D113" s="10"/>
+      <c r="E113" s="10">
         <v>4</v>
       </c>
-      <c r="F118" s="10"/>
-      <c r="G118" s="10"/>
-      <c r="H118" s="10"/>
+      <c r="F113" s="10"/>
+      <c r="G113" s="10"/>
+      <c r="H113" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="9">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 B3 C15 B30 B46 B47 B48 B53 B54 B55 B56 B60 B63 B64 B65 B66 B67 B70 B83 B84 B93 B94 B95 B96 B97 B98 B99 B100 B14:B20 B21:B29 B31:B39 B40:B45 B49:B52 B57:B59 B61:B62 B68:B69 B71:B80 B81:B82 B85:B89 B90:B91 B117:B118 C2:C3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 B3 C15 B30 B46 B47 B48 B53 B54 B55 B56 B60 B63 B64 B65 B66 B67 B70 B88 B89 B90 B91 B92 B93 B94 B95 B14:B20 B21:B29 B31:B39 B40:B45 B49:B52 B57:B59 B61:B62 B68:B69 B71:B80 B81:B82 B83:B84 B85:B86 B112:B113 C2:C3">
       <formula1>[6]DataList!#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
       <formula1>[1]DataList!#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4 C5 C6 C10 C11 C12 B13 C13 C101 B102 C102 B103 C103 B4:B12 C7:C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4 C5 C6 C10 C11 C12 B13 C13 C96 B97 C97 B98 C98 B4:B12 C7:C9">
       <formula1>[5]DataList!#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14 C16:C20 C21:C25">
@@ -4706,13 +4561,13 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C71">
       <formula1>[4]DataList!#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B101 B104:B116">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B96 B99:B111">
       <formula1/>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B119:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B114:B1048576">
       <formula1>DataList!$C$2:$C$129</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C119:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C114:C1048576">
       <formula1>DataList!$A$2:$A$11</formula1>
     </dataValidation>
   </dataValidations>
@@ -4743,7 +4598,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4751,20 +4606,20 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="C3" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -4775,20 +4630,20 @@
         <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="C6" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -4796,47 +4651,47 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="C8" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="C10" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="C11" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="3:3">
       <c r="C12" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="3:3">
       <c r="C13" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" spans="3:3">
@@ -4846,12 +4701,12 @@
     </row>
     <row r="15" spans="3:3">
       <c r="C15" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
     </row>
     <row r="16" spans="3:3">
       <c r="C16" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" spans="3:3">
@@ -4861,55 +4716,55 @@
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
     </row>
     <row r="20" spans="3:3">
       <c r="C20" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="3:3">
       <c r="C21" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="3:3">
       <c r="C22" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
     </row>
     <row r="23" spans="3:4">
       <c r="C23" s="2" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24" spans="3:3">
       <c r="C24" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
     </row>
     <row r="25" spans="3:3">
       <c r="C25" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
     </row>
     <row r="26" spans="3:3">
       <c r="C26" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
     </row>
     <row r="27" spans="3:3">
       <c r="C27" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
     </row>
     <row r="28" spans="3:3">
@@ -4919,152 +4774,152 @@
     </row>
     <row r="29" spans="3:3">
       <c r="C29" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
     </row>
     <row r="30" spans="3:3">
       <c r="C30" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
     </row>
     <row r="31" spans="3:3">
       <c r="C31" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
     </row>
     <row r="32" spans="3:3">
       <c r="C32" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="3:3">
       <c r="C33" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
     </row>
     <row r="34" spans="3:3">
       <c r="C34" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
     </row>
     <row r="35" spans="3:3">
       <c r="C35" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
     </row>
     <row r="36" spans="3:3">
       <c r="C36" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
     </row>
     <row r="37" spans="3:3">
       <c r="C37" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
     </row>
     <row r="38" spans="3:3">
       <c r="C38" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
     </row>
     <row r="39" spans="3:3">
       <c r="C39" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
     </row>
     <row r="40" spans="3:3">
       <c r="C40" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
     </row>
     <row r="41" spans="3:3">
       <c r="C41" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
     </row>
     <row r="42" spans="3:3">
       <c r="C42" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
     </row>
     <row r="43" spans="3:3">
       <c r="C43" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
     </row>
     <row r="44" spans="3:3">
       <c r="C44" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
     </row>
     <row r="45" spans="3:3">
       <c r="C45" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
     </row>
     <row r="46" spans="3:3">
       <c r="C46" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
     </row>
     <row r="47" spans="3:3">
       <c r="C47" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
     </row>
     <row r="48" spans="3:3">
       <c r="C48" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
     </row>
     <row r="49" spans="3:3">
       <c r="C49" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
     </row>
     <row r="50" spans="3:3">
       <c r="C50" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
     </row>
     <row r="51" spans="3:3">
       <c r="C51" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
     </row>
     <row r="52" spans="3:3">
       <c r="C52" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
     </row>
     <row r="53" spans="3:3">
       <c r="C53" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
     </row>
     <row r="54" spans="3:3">
       <c r="C54" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
     </row>
     <row r="55" spans="3:3">
       <c r="C55" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
     </row>
     <row r="56" spans="3:3">
       <c r="C56" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
     </row>
     <row r="57" spans="3:3">
       <c r="C57" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
     </row>
     <row r="58" spans="3:3">
       <c r="C58" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
     </row>
     <row r="59" spans="3:3">
@@ -5074,209 +4929,209 @@
     </row>
     <row r="60" spans="3:3">
       <c r="C60" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
     </row>
     <row r="61" spans="3:3">
       <c r="C61" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
     </row>
     <row r="62" spans="3:3">
       <c r="C62" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
     </row>
     <row r="63" spans="3:3">
       <c r="C63" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
     </row>
     <row r="64" spans="3:3">
       <c r="C64" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
     </row>
     <row r="65" spans="3:3">
       <c r="C65" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
     </row>
     <row r="66" spans="3:3">
       <c r="C66" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
     </row>
     <row r="67" spans="3:3">
       <c r="C67" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
     </row>
     <row r="68" spans="3:3">
       <c r="C68" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
     </row>
     <row r="69" spans="3:3">
       <c r="C69" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
     </row>
     <row r="70" spans="3:3">
       <c r="C70" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
     </row>
     <row r="71" spans="3:4">
       <c r="C71" s="2" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
     </row>
     <row r="72" spans="3:3">
       <c r="C72" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
     </row>
     <row r="73" spans="3:4">
       <c r="C73" s="2" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
     </row>
     <row r="74" spans="3:3">
       <c r="C74" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
     </row>
     <row r="75" spans="3:3">
       <c r="C75" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
     </row>
     <row r="76" spans="3:3">
       <c r="C76" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
     </row>
     <row r="77" spans="3:3">
       <c r="C77" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
     </row>
     <row r="78" spans="3:4">
       <c r="C78" s="2" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
     </row>
     <row r="79" spans="3:4">
       <c r="C79" s="2" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
     </row>
     <row r="80" spans="3:3">
       <c r="C80" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
     </row>
     <row r="81" spans="3:3">
       <c r="C81" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
     </row>
     <row r="82" spans="3:3">
       <c r="C82" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
     </row>
     <row r="83" spans="3:3">
       <c r="C83" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
     </row>
     <row r="84" spans="3:3">
       <c r="C84" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
     </row>
     <row r="85" spans="3:3">
       <c r="C85" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
     </row>
     <row r="86" spans="3:3">
       <c r="C86" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
     </row>
     <row r="87" spans="3:3">
       <c r="C87" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
     </row>
     <row r="88" spans="3:3">
       <c r="C88" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
     </row>
     <row r="89" spans="3:3">
       <c r="C89" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
     </row>
     <row r="90" spans="3:3">
       <c r="C90" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
     </row>
     <row r="91" spans="3:3">
       <c r="C91" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
     </row>
     <row r="92" spans="3:3">
       <c r="C92" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
     </row>
     <row r="93" spans="3:3">
       <c r="C93" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
     </row>
     <row r="94" spans="3:3">
       <c r="C94" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
     </row>
     <row r="95" spans="3:3">
       <c r="C95" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
     </row>
     <row r="96" spans="3:3">
       <c r="C96" s="3" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
     </row>
     <row r="97" spans="3:3">
       <c r="C97" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
     </row>
     <row r="98" spans="3:3">
       <c r="C98" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
     </row>
     <row r="99" spans="3:3">
@@ -5286,7 +5141,7 @@
     </row>
     <row r="100" spans="3:3">
       <c r="C100" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>